<commit_message>
DCF integration and the odd change
</commit_message>
<xml_diff>
--- a/models/3_Statement_Model.xlsx
+++ b/models/3_Statement_Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xavie\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb10f4a09bcef627/Documents/GitHub/XD_Grad_Portfolio/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2465401F-8E98-4D2A-899A-91CC703B4779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{2465401F-8E98-4D2A-899A-91CC703B4779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88D7CCC9-6E5D-4E71-AB39-7360AF481212}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Income Statement" sheetId="5" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
   <si>
     <t>Notes</t>
   </si>
@@ -279,9 +279,6 @@
     <t>Short Term Debt</t>
   </si>
   <si>
-    <t>Current Portion of Long Term Debt</t>
-  </si>
-  <si>
     <t>Current Portion of Leases</t>
   </si>
   <si>
@@ -424,6 +421,15 @@
   </si>
   <si>
     <t>Other Financing Activities</t>
+  </si>
+  <si>
+    <t>Net Working Capital</t>
+  </si>
+  <si>
+    <t>Change in NWC</t>
+  </si>
+  <si>
+    <t>Current Portion of Long-Term Debt</t>
   </si>
 </sst>
 </file>
@@ -1089,11 +1095,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1219,7 +1225,7 @@
         <v>-2337.4090669735197</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N3" s="57">
         <f>((5.15*350)+(5.4*650))/1000/100</f>
@@ -1271,7 +1277,7 @@
         <v>5560.0497594532026</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N4" s="66">
         <v>0.05</v>
@@ -1317,7 +1323,7 @@
         <v>-4059.9988391784418</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N5" s="57">
         <v>1.2999999999999999E-2</v>
@@ -1363,7 +1369,7 @@
         <v>-392.83401047113989</v>
       </c>
       <c r="M6" s="53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N6" s="57">
         <v>0.66600000000000004</v>
@@ -1480,23 +1486,23 @@
       </c>
       <c r="G9" s="25">
         <f>-$N$3*'Balance Sheet'!F49</f>
-        <v>-133.13125000000002</v>
+        <v>-158.63125000000002</v>
       </c>
       <c r="H9" s="25">
         <f>-$N$3*'Balance Sheet'!G49</f>
-        <v>-134.85853740352562</v>
+        <v>-161.61118381490064</v>
       </c>
       <c r="I9" s="25">
         <f>-$N$3*'Balance Sheet'!H49</f>
-        <v>-135.72880605349886</v>
+        <v>-163.80822056441863</v>
       </c>
       <c r="J9" s="25">
         <f>-$N$3*'Balance Sheet'!I49</f>
-        <v>-135.20278979475705</v>
+        <v>-164.68747799913208</v>
       </c>
       <c r="K9" s="25">
         <f>-$N$3*'Balance Sheet'!J49</f>
-        <v>-133.04135243697249</v>
+        <v>-164.01446309356677</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1524,19 +1530,19 @@
       </c>
       <c r="H10" s="25">
         <f>'Balance Sheet'!G3*'Income Statement'!$N$5</f>
-        <v>7.6243226118431435</v>
+        <v>7.3278538743431456</v>
       </c>
       <c r="I10" s="25">
         <f>'Balance Sheet'!H3*'Income Statement'!$N$5</f>
-        <v>5.3814127539673384</v>
+        <v>4.7704649176956107</v>
       </c>
       <c r="J10" s="25">
         <f>'Balance Sheet'!I3*'Income Statement'!$N$5</f>
-        <v>3.5816795266947379</v>
+        <v>2.6371710824430332</v>
       </c>
       <c r="K10" s="25">
         <f>'Balance Sheet'!J3*'Income Statement'!$N$5</f>
-        <v>2.2785660874820253</v>
+        <v>0.98028095642414315</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1646,23 +1652,23 @@
       </c>
       <c r="G13" s="26">
         <f t="shared" ref="G13" si="12">SUM(G8:G12)</f>
-        <v>700.12749197145445</v>
+        <v>674.62749197145445</v>
       </c>
       <c r="H13" s="26">
         <f t="shared" ref="H13" si="13">SUM(H8:H12)</f>
-        <v>752.626968115468</v>
+        <v>725.57785296659301</v>
       </c>
       <c r="I13" s="26">
         <f t="shared" ref="I13" si="14">SUM(I8:I12)</f>
-        <v>807.79324555503899</v>
+        <v>779.10288320784741</v>
       </c>
       <c r="J13" s="26">
         <f t="shared" ref="J13" si="15">SUM(J8:J12)</f>
-        <v>868.6812771749735</v>
+        <v>838.25208052634684</v>
       </c>
       <c r="K13" s="26">
         <f t="shared" ref="K13" si="16">SUM(K8:K12)</f>
-        <v>935.85412345413056</v>
+        <v>903.58272766647849</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1881,23 +1887,23 @@
       </c>
       <c r="G19" s="26">
         <f t="shared" ref="G19" si="21">SUM(G13:G18)</f>
-        <v>435.52749197145442</v>
+        <v>410.02749197145448</v>
       </c>
       <c r="H19" s="26">
         <f t="shared" ref="H19" si="22">SUM(H13:H18)</f>
-        <v>488.02696811546798</v>
+        <v>460.97785296659299</v>
       </c>
       <c r="I19" s="26">
         <f t="shared" ref="I19" si="23">SUM(I13:I18)</f>
-        <v>543.19324555503897</v>
+        <v>514.50288320784739</v>
       </c>
       <c r="J19" s="26">
         <f t="shared" ref="J19" si="24">SUM(J13:J18)</f>
-        <v>604.08127717497348</v>
+        <v>573.65208052634682</v>
       </c>
       <c r="K19" s="26">
         <f t="shared" ref="K19" si="25">SUM(K13:K18)</f>
-        <v>671.25412345413054</v>
+        <v>638.98272766647847</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -1921,23 +1927,23 @@
       </c>
       <c r="G20" s="25">
         <f>G19*G36</f>
-        <v>46.024367714083439</v>
+        <v>43.329655214083452</v>
       </c>
       <c r="H20" s="25">
         <f t="shared" ref="H20:K20" si="26">H19*H36</f>
-        <v>51.572249855602074</v>
+        <v>48.71383461224471</v>
       </c>
       <c r="I20" s="25">
         <f t="shared" si="26"/>
-        <v>57.401946224028741</v>
+        <v>54.370092182989268</v>
       </c>
       <c r="J20" s="25">
         <f t="shared" si="26"/>
-        <v>63.836288965465315</v>
+        <v>60.620683609621693</v>
       </c>
       <c r="K20" s="25">
         <f t="shared" si="26"/>
-        <v>70.934779496015238</v>
+        <v>67.524499746155101</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -1966,23 +1972,23 @@
       </c>
       <c r="G21" s="26">
         <f>G19-G20</f>
-        <v>389.50312425737098</v>
+        <v>366.69783675737102</v>
       </c>
       <c r="H21" s="26">
         <f t="shared" ref="H21:K21" si="28">H19-H20</f>
-        <v>436.4547182598659</v>
+        <v>412.26401835434831</v>
       </c>
       <c r="I21" s="26">
         <f t="shared" si="28"/>
-        <v>485.79129933101024</v>
+        <v>460.13279102485814</v>
       </c>
       <c r="J21" s="26">
         <f t="shared" si="28"/>
-        <v>540.24498820950816</v>
+        <v>513.03139691672516</v>
       </c>
       <c r="K21" s="26">
         <f t="shared" si="28"/>
-        <v>600.31934395811527</v>
+        <v>571.45822792032334</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2010,23 +2016,23 @@
       </c>
       <c r="G22" s="28">
         <f t="shared" ref="G22" si="30">(G21-F21)/F21</f>
-        <v>-5.4604067336478192E-2</v>
+        <v>-0.10995670689958489</v>
       </c>
       <c r="H22" s="28">
         <f t="shared" ref="H22" si="31">(H21-G21)/G21</f>
-        <v>0.12054227829882778</v>
+        <v>0.1242608410235225</v>
       </c>
       <c r="I22" s="28">
         <f t="shared" ref="I22" si="32">(I21-H21)/H21</f>
-        <v>0.11303940364729716</v>
+        <v>0.11611193443849314</v>
       </c>
       <c r="J22" s="28">
         <f t="shared" ref="J22" si="33">(J21-I21)/I21</f>
-        <v>0.11209276278411499</v>
+        <v>0.11496378202919522</v>
       </c>
       <c r="K22" s="28">
         <f t="shared" ref="K22" si="34">(K21-J21)/J21</f>
-        <v>0.11119835826280751</v>
+        <v>0.11388548801250457</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -2205,23 +2211,23 @@
       </c>
       <c r="G28" s="69">
         <f t="shared" si="39"/>
-        <v>0.44616623626273882</v>
+        <v>0.42004334107373542</v>
       </c>
       <c r="H28" s="69">
         <f t="shared" ref="H28:K28" si="40">H21/H24</f>
-        <v>0.49994813088186241</v>
+        <v>0.4722382799018881</v>
       </c>
       <c r="I28" s="69">
         <f t="shared" si="40"/>
-        <v>0.55646196945132897</v>
+        <v>0.52707078009720287</v>
       </c>
       <c r="J28" s="69">
         <f t="shared" si="40"/>
-        <v>0.6188373289914183</v>
+        <v>0.58766483037425565</v>
       </c>
       <c r="K28" s="69">
         <f t="shared" si="40"/>
-        <v>0.68765102400700484</v>
+        <v>0.65459132636921347</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -2250,23 +2256,23 @@
       </c>
       <c r="G29" s="70">
         <f t="shared" si="41"/>
-        <v>0.44463826970019521</v>
+        <v>0.41860483648101715</v>
       </c>
       <c r="H29" s="70">
         <f t="shared" ref="H29:K29" si="42">H21/H25</f>
-        <v>0.49823597974870537</v>
+        <v>0.47062102551866247</v>
       </c>
       <c r="I29" s="70">
         <f t="shared" si="42"/>
-        <v>0.55455627777512584</v>
+        <v>0.52526574317906183</v>
       </c>
       <c r="J29" s="70">
         <f t="shared" si="42"/>
-        <v>0.61671802307021484</v>
+        <v>0.58565227958530264</v>
       </c>
       <c r="K29" s="70">
         <f t="shared" si="42"/>
-        <v>0.68529605474670696</v>
+        <v>0.6523495752515106</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -2890,11 +2896,11 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:R215"/>
+  <dimension ref="A1:R216"/>
   <sheetViews>
-    <sheetView showGridLines="0" showWhiteSpace="0" topLeftCell="A17" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showWhiteSpace="0" topLeftCell="A22" zoomScale="91" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C35" sqref="C35"/>
+      <selection pane="topRight" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2981,23 +2987,23 @@
       </c>
       <c r="G3" s="25">
         <f>F3+'Cash Flow'!B29</f>
-        <v>586.48635475716492</v>
+        <v>563.68106725716507</v>
       </c>
       <c r="H3" s="25">
         <f>G3+'Cash Flow'!C29</f>
-        <v>413.95482722825682</v>
+        <v>366.95883982273926</v>
       </c>
       <c r="I3" s="25">
         <f>H3+'Cash Flow'!D29</f>
-        <v>275.51380974574909</v>
+        <v>202.85931403407949</v>
       </c>
       <c r="J3" s="25">
         <f>I3+'Cash Flow'!E29</f>
-        <v>175.27431442169427</v>
+        <v>75.40622741724178</v>
       </c>
       <c r="K3" s="25">
         <f>J3+'Cash Flow'!F29</f>
-        <v>118.02176967337527</v>
+        <v>-10.70743336886926</v>
       </c>
       <c r="L3" s="12"/>
     </row>
@@ -3101,7 +3107,7 @@
       </c>
       <c r="L5" s="12"/>
       <c r="M5" s="55" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N5" s="54">
         <f>'Income Statement'!G32</f>
@@ -3170,7 +3176,7 @@
       </c>
       <c r="L6" s="12"/>
       <c r="M6" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N6" s="54">
         <f>('Income Statement'!G3-'Income Statement'!F3)/'Income Statement'!F3</f>
@@ -3234,7 +3240,7 @@
       </c>
       <c r="L7" s="12"/>
       <c r="M7" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N7" s="54">
         <f>'Income Statement'!G36</f>
@@ -3377,23 +3383,23 @@
       </c>
       <c r="G10" s="26">
         <f t="shared" si="2"/>
-        <v>4610.9890374407423</v>
+        <v>4588.183749940742</v>
       </c>
       <c r="H10" s="26">
         <f t="shared" si="2"/>
-        <v>4692.4813478792785</v>
+        <v>4645.4853604737618</v>
       </c>
       <c r="I10" s="26">
         <f t="shared" si="2"/>
-        <v>4824.937357355162</v>
+        <v>4752.2828616434927</v>
       </c>
       <c r="J10" s="26">
         <f t="shared" si="2"/>
-        <v>5013.6407255050308</v>
+        <v>4913.7726385005781</v>
       </c>
       <c r="K10" s="26">
         <f t="shared" si="2"/>
-        <v>5264.6341425559367</v>
+        <v>5135.9049395136917</v>
       </c>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
@@ -3423,23 +3429,23 @@
         <v>1422</v>
       </c>
       <c r="G11" s="25">
-        <f>F11-G52-'Income Statement'!G39</f>
+        <f>F11-G53-'Income Statement'!G39</f>
         <v>1425.3978586658409</v>
       </c>
       <c r="H11" s="25">
-        <f>G11-H52-'Income Statement'!H39</f>
+        <f>G11-H53-'Income Statement'!H39</f>
         <v>1429.0101878308276</v>
       </c>
       <c r="I11" s="25">
-        <f>H11-I52-'Income Statement'!I39</f>
+        <f>H11-I53-'Income Statement'!I39</f>
         <v>1432.851233407052</v>
       </c>
       <c r="J11" s="25">
-        <f>I11-J52-'Income Statement'!J39</f>
+        <f>I11-J53-'Income Statement'!J39</f>
         <v>1436.9362313644767</v>
       </c>
       <c r="K11" s="25">
-        <f>J11-K52-'Income Statement'!K39</f>
+        <f>J11-K53-'Income Statement'!K39</f>
         <v>1441.2814791701667</v>
       </c>
       <c r="L11" s="12"/>
@@ -3626,7 +3632,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="12">
         <v>166</v>
@@ -3668,7 +3674,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="14">
         <f t="shared" ref="B17:K17" si="7">SUM(B11:B16)</f>
@@ -3739,23 +3745,23 @@
       </c>
       <c r="G18" s="26">
         <f t="shared" si="8"/>
-        <v>10494.468624204976</v>
+        <v>10471.663336704976</v>
       </c>
       <c r="H18" s="26">
         <f t="shared" si="8"/>
-        <v>10538.395706761647</v>
+        <v>10491.39971935613</v>
       </c>
       <c r="I18" s="26">
         <f t="shared" si="8"/>
-        <v>10644.98663721863</v>
+        <v>10572.332141506962</v>
       </c>
       <c r="J18" s="26">
         <f t="shared" si="8"/>
-        <v>10819.374117177293</v>
+        <v>10719.506030172841</v>
       </c>
       <c r="K18" s="26">
         <f t="shared" si="8"/>
-        <v>11067.553462829319</v>
+        <v>10938.824259787074</v>
       </c>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
@@ -3873,7 +3879,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="B23" s="12">
         <v>268</v>
@@ -3915,7 +3921,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="12">
         <v>58</v>
@@ -3957,7 +3963,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" s="12">
         <v>206</v>
@@ -4005,7 +4011,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="12">
         <v>254</v>
@@ -4053,7 +4059,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="14">
         <f>SUM(B21:B26)</f>
@@ -4100,7 +4106,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28" s="12">
         <v>3207</v>
@@ -4142,7 +4148,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" s="12">
         <v>146</v>
@@ -4184,7 +4190,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="12">
         <v>163</v>
@@ -4226,7 +4232,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="12">
         <v>141</v>
@@ -4263,7 +4269,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="12">
         <v>388</v>
@@ -4305,7 +4311,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="14">
         <f>SUM(B28:B32)</f>
@@ -4352,7 +4358,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="14">
         <f>B33+B27</f>
@@ -4414,7 +4420,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -4431,7 +4437,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37" s="12">
         <v>177</v>
@@ -4473,7 +4479,7 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" s="12">
         <v>612</v>
@@ -4515,7 +4521,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B39" s="12">
         <v>4958</v>
@@ -4533,31 +4539,31 @@
         <v>5018</v>
       </c>
       <c r="G39" s="25">
-        <f>F39+'Income Statement'!G21+G54</f>
-        <v>5080.5031242573714</v>
+        <f>F39+'Income Statement'!G21+G55</f>
+        <v>5057.6978367573711</v>
       </c>
       <c r="H39" s="25">
-        <f>G39+'Income Statement'!H21+H54</f>
-        <v>5189.9578425172376</v>
+        <f>G39+'Income Statement'!H21+H55</f>
+        <v>5142.9618551117192</v>
       </c>
       <c r="I39" s="25">
-        <f>H39+'Income Statement'!I21+I54</f>
-        <v>5348.7491418482477</v>
+        <f>H39+'Income Statement'!I21+I55</f>
+        <v>5276.0946461365775</v>
       </c>
       <c r="J39" s="25">
-        <f>I39+'Income Statement'!J21+J54</f>
-        <v>5561.9941300577557</v>
+        <f>I39+'Income Statement'!J21+J55</f>
+        <v>5462.126043053303</v>
       </c>
       <c r="K39" s="25">
-        <f>J39+'Income Statement'!K21+K54</f>
-        <v>5835.3134740158712</v>
+        <f>J39+'Income Statement'!K21+K55</f>
+        <v>5706.5842709736262</v>
       </c>
       <c r="L39" s="12"/>
       <c r="M39" s="12"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40" s="12">
         <v>-157</v>
@@ -4599,7 +4605,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B41" s="12">
         <v>-311</v>
@@ -4641,7 +4647,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B42" s="14">
         <f>SUM(B37:B41)</f>
@@ -4665,23 +4671,23 @@
       </c>
       <c r="G42" s="26">
         <f t="shared" si="34"/>
-        <v>5327.5031242573714</v>
+        <v>5304.6978367573711</v>
       </c>
       <c r="H42" s="26">
         <f t="shared" ref="H42" si="35">SUM(H37:H41)</f>
-        <v>5436.9578425172376</v>
+        <v>5389.9618551117192</v>
       </c>
       <c r="I42" s="26">
         <f t="shared" ref="I42" si="36">SUM(I37:I41)</f>
-        <v>5595.7491418482477</v>
+        <v>5523.0946461365775</v>
       </c>
       <c r="J42" s="26">
         <f t="shared" ref="J42" si="37">SUM(J37:J41)</f>
-        <v>5808.9941300577557</v>
+        <v>5709.126043053303</v>
       </c>
       <c r="K42" s="26">
         <f t="shared" ref="K42" si="38">SUM(K37:K41)</f>
-        <v>6082.3134740158712</v>
+        <v>5953.5842709736262</v>
       </c>
       <c r="L42" s="12"/>
       <c r="M42" s="12"/>
@@ -4703,7 +4709,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B44" s="52">
         <f>B18-(B34+B42)</f>
@@ -4727,7 +4733,7 @@
       </c>
       <c r="G44" s="56">
         <f t="shared" si="39"/>
-        <v>5.3399245753098512E-3</v>
+        <v>5.3399245771288406E-3</v>
       </c>
       <c r="H44" s="56">
         <f t="shared" si="39"/>
@@ -4735,11 +4741,11 @@
       </c>
       <c r="I44" s="56">
         <f t="shared" si="39"/>
-        <v>0.19023507950623753</v>
+        <v>0.19023507950805651</v>
       </c>
       <c r="J44" s="56">
         <f t="shared" si="39"/>
-        <v>2.5465767974310438E-2</v>
+        <v>2.5465767976129428E-2</v>
       </c>
       <c r="K44" s="56">
         <f t="shared" si="39"/>
@@ -4778,7 +4784,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -4818,77 +4824,77 @@
       </c>
       <c r="G48" s="42">
         <f t="shared" ref="G48:K48" si="40">(G3-F3)/F3</f>
-        <v>-5.2526082783255386E-2</v>
+        <v>-8.9368227371300374E-2</v>
       </c>
       <c r="H48" s="42">
         <f t="shared" si="40"/>
-        <v>-0.2941782466539139</v>
+        <v>-0.3489956268917514</v>
       </c>
       <c r="I48" s="42">
         <f t="shared" si="40"/>
-        <v>-0.33443508415996959</v>
+        <v>-0.44718782593690515</v>
       </c>
       <c r="J48" s="42">
         <f t="shared" si="40"/>
-        <v>-0.36382748079509442</v>
+        <v>-0.62828313909917954</v>
       </c>
       <c r="K48" s="42">
         <f t="shared" si="40"/>
-        <v>-0.32664537834433921</v>
+        <v>-1.1419966723652983</v>
       </c>
       <c r="L48" s="12"/>
       <c r="M48" s="12"/>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" s="12">
-        <f>B22+B28+B23-B3</f>
-        <v>1724</v>
+        <f>B22+B28+B23-B3-B12+B24+B30+B29+B31+B32</f>
+        <v>2503</v>
       </c>
       <c r="C49" s="12">
-        <f t="shared" ref="C49:K49" si="41">C22+C28+C23-C3</f>
-        <v>1852</v>
+        <f t="shared" ref="C49:E49" si="41">C22+C28+C23-C3-C12+C24+C30+C29+C31+C32</f>
+        <v>2224</v>
       </c>
       <c r="D49" s="12">
         <f t="shared" si="41"/>
-        <v>2326</v>
+        <v>2744</v>
       </c>
       <c r="E49" s="12">
         <f t="shared" si="41"/>
-        <v>2583</v>
+        <v>2938</v>
       </c>
       <c r="F49" s="12">
-        <f t="shared" si="41"/>
-        <v>2506</v>
+        <f>F22+F28+F23-F3-F12+F24+F30+F29+F31+F32</f>
+        <v>2986</v>
       </c>
       <c r="G49" s="25">
-        <f t="shared" si="41"/>
-        <v>2538.5136452428351</v>
+        <f t="shared" ref="G49:K49" si="42">G22+G28+G23-G3-G12+G24+G30+G29+G31+G32</f>
+        <v>3042.0928718098939</v>
       </c>
       <c r="H49" s="25">
-        <f t="shared" si="41"/>
-        <v>2554.8951727717431</v>
+        <f t="shared" si="42"/>
+        <v>3083.4488576831741</v>
       </c>
       <c r="I49" s="25">
-        <f t="shared" si="41"/>
-        <v>2544.9936902542504</v>
+        <f t="shared" si="42"/>
+        <v>3099.9995858660154</v>
       </c>
       <c r="J49" s="25">
-        <f t="shared" si="41"/>
-        <v>2504.3078105783056</v>
+        <f t="shared" si="42"/>
+        <v>3087.3310699965509</v>
       </c>
       <c r="K49" s="25">
-        <f t="shared" si="41"/>
-        <v>2427.6812490766247</v>
+        <f t="shared" si="42"/>
+        <v>3040.379594930776</v>
       </c>
       <c r="L49" s="12"/>
       <c r="M49" s="12"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B50" s="41">
         <f>'Income Statement'!B2/'Balance Sheet'!B18</f>
@@ -4912,190 +4918,253 @@
       </c>
       <c r="G50" s="42">
         <f>'Income Statement'!G2/'Balance Sheet'!G18</f>
-        <v>0.58846099044166733</v>
+        <v>0.58974254635480639</v>
       </c>
       <c r="H50" s="42">
         <f>'Income Statement'!H2/'Balance Sheet'!H18</f>
-        <v>0.6229965434296918</v>
+        <v>0.62578724233468974</v>
       </c>
       <c r="I50" s="42">
         <f>'Income Statement'!I2/'Balance Sheet'!I18</f>
-        <v>0.65580868105554624</v>
+        <v>0.66031548696815667</v>
       </c>
       <c r="J50" s="42">
         <f>'Income Statement'!J2/'Balance Sheet'!J18</f>
-        <v>0.68621866545245058</v>
+        <v>0.69261180942686362</v>
       </c>
       <c r="K50" s="42">
         <f>'Income Statement'!K2/'Balance Sheet'!K18</f>
-        <v>0.71356861775735292</v>
+        <v>0.72196596625645471</v>
       </c>
       <c r="L50" s="12"/>
       <c r="M50" s="12"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="25"/>
+      <c r="A51" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" s="12">
+        <f>B6+B7+B8-B21-B26</f>
+        <v>1733</v>
+      </c>
+      <c r="C51" s="12">
+        <f t="shared" ref="C51:K51" si="43">C6+C7+C8-C21-C26</f>
+        <v>1677</v>
+      </c>
+      <c r="D51" s="12">
+        <f t="shared" si="43"/>
+        <v>2118</v>
+      </c>
+      <c r="E51" s="12">
+        <f t="shared" si="43"/>
+        <v>2413</v>
+      </c>
+      <c r="F51" s="12">
+        <f t="shared" si="43"/>
+        <v>2519</v>
+      </c>
+      <c r="G51" s="25">
+        <f t="shared" si="43"/>
+        <v>2668.3564581161982</v>
+      </c>
+      <c r="H51" s="25">
+        <f t="shared" si="43"/>
+        <v>2836.7812802619032</v>
+      </c>
+      <c r="I51" s="25">
+        <f t="shared" si="43"/>
+        <v>3016.3934928413955</v>
+      </c>
+      <c r="J51" s="25">
+        <f t="shared" si="43"/>
+        <v>3207.9705935586248</v>
+      </c>
+      <c r="K51" s="25">
+        <f t="shared" si="43"/>
+        <v>3412.3461817261409</v>
+      </c>
       <c r="L51" s="12"/>
       <c r="M51" s="12"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="12" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="B52" s="12">
-        <v>-443</v>
+        <v>0</v>
       </c>
       <c r="C52" s="12">
-        <v>-408</v>
+        <f>C51-B51</f>
+        <v>-56</v>
       </c>
       <c r="D52" s="12">
-        <v>-358</v>
+        <f t="shared" ref="D52:K52" si="44">D51-C51</f>
+        <v>441</v>
       </c>
       <c r="E52" s="12">
-        <v>-427</v>
+        <f t="shared" si="44"/>
+        <v>295</v>
       </c>
       <c r="F52" s="12">
-        <v>-381</v>
+        <f t="shared" si="44"/>
+        <v>106</v>
       </c>
       <c r="G52" s="25">
-        <f>-G53*'Income Statement'!G2</f>
-        <v>-477.50310262561572</v>
+        <f t="shared" si="44"/>
+        <v>149.35645811619816</v>
       </c>
       <c r="H52" s="25">
-        <f>-H53*'Income Statement'!H2</f>
-        <v>-507.64276964391172</v>
+        <f t="shared" si="44"/>
+        <v>168.42482214570509</v>
       </c>
       <c r="I52" s="25">
-        <f>-I53*'Income Statement'!I2</f>
-        <v>-539.78442317572933</v>
+        <f t="shared" si="44"/>
+        <v>179.61221257949228</v>
       </c>
       <c r="J52" s="25">
-        <f>-J53*'Income Statement'!J2</f>
-        <v>-574.06719664336379</v>
+        <f t="shared" si="44"/>
+        <v>191.57710071722931</v>
       </c>
       <c r="K52" s="25">
-        <f>-K53*'Income Statement'!K2</f>
-        <v>-610.64026286698993</v>
+        <f t="shared" si="44"/>
+        <v>204.37558816751607</v>
       </c>
       <c r="L52" s="12"/>
       <c r="M52" s="12"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="B53" s="41">
-        <f>-B52/'Income Statement'!B2</f>
-        <v>9.7149122807017541E-2</v>
-      </c>
-      <c r="C53" s="41">
-        <f>-C52/'Income Statement'!C2</f>
-        <v>7.8280890253261709E-2</v>
-      </c>
-      <c r="D53" s="41">
-        <f>-D52/'Income Statement'!D2</f>
-        <v>6.8648130393096835E-2</v>
-      </c>
-      <c r="E53" s="41">
-        <f>-E52/'Income Statement'!E2</f>
-        <v>7.6950801946296624E-2</v>
-      </c>
-      <c r="F53" s="41">
-        <f>-F52/'Income Statement'!F2</f>
-        <v>6.5576592082616181E-2</v>
-      </c>
-      <c r="G53" s="42">
-        <f>AVERAGE($B$53:$F$53)</f>
-        <v>7.7321107496457778E-2</v>
-      </c>
-      <c r="H53" s="42">
-        <f t="shared" ref="H53:K53" si="42">AVERAGE($B$53:$F$53)</f>
-        <v>7.7321107496457778E-2</v>
-      </c>
-      <c r="I53" s="42">
-        <f t="shared" si="42"/>
-        <v>7.7321107496457778E-2</v>
-      </c>
-      <c r="J53" s="42">
-        <f t="shared" si="42"/>
-        <v>7.7321107496457778E-2</v>
-      </c>
-      <c r="K53" s="42">
-        <f t="shared" si="42"/>
-        <v>7.7321107496457778E-2</v>
+        <v>99</v>
+      </c>
+      <c r="B53" s="12">
+        <v>-443</v>
+      </c>
+      <c r="C53" s="12">
+        <v>-408</v>
+      </c>
+      <c r="D53" s="12">
+        <v>-358</v>
+      </c>
+      <c r="E53" s="12">
+        <v>-427</v>
+      </c>
+      <c r="F53" s="12">
+        <v>-381</v>
+      </c>
+      <c r="G53" s="25">
+        <f>-G54*'Income Statement'!G2</f>
+        <v>-477.50310262561572</v>
+      </c>
+      <c r="H53" s="25">
+        <f>-H54*'Income Statement'!H2</f>
+        <v>-507.64276964391172</v>
+      </c>
+      <c r="I53" s="25">
+        <f>-I54*'Income Statement'!I2</f>
+        <v>-539.78442317572933</v>
+      </c>
+      <c r="J53" s="25">
+        <f>-J54*'Income Statement'!J2</f>
+        <v>-574.06719664336379</v>
+      </c>
+      <c r="K53" s="25">
+        <f>-K54*'Income Statement'!K2</f>
+        <v>-610.64026286698993</v>
       </c>
       <c r="L53" s="12"/>
       <c r="M53" s="12"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B54" s="12">
-        <v>-328</v>
-      </c>
-      <c r="C54" s="12">
-        <v>-329</v>
-      </c>
-      <c r="D54" s="12">
-        <v>-327</v>
-      </c>
-      <c r="E54" s="12">
-        <v>-327</v>
-      </c>
-      <c r="F54" s="12">
-        <v>-327</v>
-      </c>
-      <c r="G54" s="25">
-        <v>-327</v>
-      </c>
-      <c r="H54" s="25">
-        <v>-327</v>
-      </c>
-      <c r="I54" s="25">
-        <v>-327</v>
-      </c>
-      <c r="J54" s="25">
-        <v>-327</v>
-      </c>
-      <c r="K54" s="25">
-        <v>-327</v>
+        <v>100</v>
+      </c>
+      <c r="B54" s="41">
+        <f>-B53/'Income Statement'!B2</f>
+        <v>9.7149122807017541E-2</v>
+      </c>
+      <c r="C54" s="41">
+        <f>-C53/'Income Statement'!C2</f>
+        <v>7.8280890253261709E-2</v>
+      </c>
+      <c r="D54" s="41">
+        <f>-D53/'Income Statement'!D2</f>
+        <v>6.8648130393096835E-2</v>
+      </c>
+      <c r="E54" s="41">
+        <f>-E53/'Income Statement'!E2</f>
+        <v>7.6950801946296624E-2</v>
+      </c>
+      <c r="F54" s="41">
+        <f>-F53/'Income Statement'!F2</f>
+        <v>6.5576592082616181E-2</v>
+      </c>
+      <c r="G54" s="42">
+        <f>AVERAGE($B$54:$F$54)</f>
+        <v>7.7321107496457778E-2</v>
+      </c>
+      <c r="H54" s="42">
+        <f t="shared" ref="H54:K54" si="45">AVERAGE($B$54:$F$54)</f>
+        <v>7.7321107496457778E-2</v>
+      </c>
+      <c r="I54" s="42">
+        <f t="shared" si="45"/>
+        <v>7.7321107496457778E-2</v>
+      </c>
+      <c r="J54" s="42">
+        <f t="shared" si="45"/>
+        <v>7.7321107496457778E-2</v>
+      </c>
+      <c r="K54" s="42">
+        <f t="shared" si="45"/>
+        <v>7.7321107496457778E-2</v>
       </c>
       <c r="L54" s="12"/>
       <c r="M54" s="12"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A55" s="12"/>
-      <c r="B55" s="41"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="41"/>
-      <c r="G55" s="68"/>
-      <c r="H55" s="68"/>
-      <c r="I55" s="68"/>
-      <c r="J55" s="68"/>
-      <c r="K55" s="68"/>
+      <c r="A55" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" s="12">
+        <v>-328</v>
+      </c>
+      <c r="C55" s="12">
+        <v>-329</v>
+      </c>
+      <c r="D55" s="12">
+        <v>-327</v>
+      </c>
+      <c r="E55" s="12">
+        <v>-327</v>
+      </c>
+      <c r="F55" s="12">
+        <v>-327</v>
+      </c>
+      <c r="G55" s="25">
+        <v>-327</v>
+      </c>
+      <c r="H55" s="25">
+        <v>-327</v>
+      </c>
+      <c r="I55" s="25">
+        <v>-327</v>
+      </c>
+      <c r="J55" s="25">
+        <v>-327</v>
+      </c>
+      <c r="K55" s="25">
+        <v>-327</v>
+      </c>
       <c r="L55" s="12"/>
       <c r="M55" s="12"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="12"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="12"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
+      <c r="B56" s="41"/>
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
       <c r="G56" s="68"/>
       <c r="H56" s="68"/>
       <c r="I56" s="68"/>
@@ -5255,6 +5324,7 @@
       <c r="M66" s="12"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A67" s="12"/>
       <c r="B67" s="12"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
@@ -5283,7 +5353,6 @@
       <c r="M68" s="12"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A69" s="12"/>
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
@@ -7473,8 +7542,23 @@
       <c r="M214" s="12"/>
     </row>
     <row r="215" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A215" s="12"/>
+      <c r="B215" s="12"/>
+      <c r="C215" s="12"/>
+      <c r="D215" s="12"/>
+      <c r="E215" s="12"/>
+      <c r="F215" s="12"/>
+      <c r="G215" s="68"/>
+      <c r="H215" s="68"/>
+      <c r="I215" s="68"/>
+      <c r="J215" s="68"/>
+      <c r="K215" s="68"/>
       <c r="L215" s="12"/>
       <c r="M215" s="12"/>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="L216" s="12"/>
+      <c r="M216" s="12"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G1:K21">
@@ -7503,8 +7587,8 @@
   <dimension ref="A1:H214"/>
   <sheetViews>
     <sheetView showGridLines="0" showWhiteSpace="0" zoomScale="90" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7537,7 +7621,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="50" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -7552,23 +7636,23 @@
       </c>
       <c r="B3" s="26">
         <f>'Income Statement'!G21</f>
-        <v>389.50312425737098</v>
+        <v>366.69783675737102</v>
       </c>
       <c r="C3" s="26">
         <f>'Income Statement'!H21</f>
-        <v>436.4547182598659</v>
+        <v>412.26401835434831</v>
       </c>
       <c r="D3" s="26">
         <f>'Income Statement'!I21</f>
-        <v>485.79129933101024</v>
+        <v>460.13279102485814</v>
       </c>
       <c r="E3" s="26">
         <f>'Income Statement'!J21</f>
-        <v>540.24498820950816</v>
+        <v>513.03139691672516</v>
       </c>
       <c r="F3" s="26">
         <f>'Income Statement'!K21</f>
-        <v>600.31934395811527</v>
+        <v>571.45822792032334</v>
       </c>
       <c r="G3" s="12"/>
     </row>
@@ -7730,7 +7814,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="25">
         <f>'Balance Sheet'!G25-'Balance Sheet'!F25</f>
@@ -7756,7 +7840,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="25">
         <f>'Balance Sheet'!G26-'Balance Sheet'!F26</f>
@@ -7782,27 +7866,27 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="26">
         <f>SUM(B3:B11)</f>
-        <v>729.74397928438839</v>
+        <v>706.93869178438854</v>
       </c>
       <c r="C12" s="26">
         <f t="shared" ref="C12:F12" si="0">SUM(C3:C11)</f>
-        <v>788.32607113060703</v>
+        <v>764.13537122508933</v>
       </c>
       <c r="D12" s="26">
         <f t="shared" si="0"/>
-        <v>859.20723228489123</v>
+        <v>833.54872397873919</v>
       </c>
       <c r="E12" s="26">
         <f t="shared" si="0"/>
-        <v>936.60225606984955</v>
+        <v>909.38866477706665</v>
       </c>
       <c r="F12" s="26">
         <f t="shared" si="0"/>
-        <v>1021.1099259891853</v>
+        <v>992.24880995139324</v>
       </c>
       <c r="G12" s="12"/>
     </row>
@@ -7817,7 +7901,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
@@ -7828,33 +7912,33 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B15" s="25">
-        <f>'Balance Sheet'!G52</f>
+        <f>'Balance Sheet'!G53</f>
         <v>-477.50310262561572</v>
       </c>
       <c r="C15" s="25">
-        <f>'Balance Sheet'!H52</f>
+        <f>'Balance Sheet'!H53</f>
         <v>-507.64276964391172</v>
       </c>
       <c r="D15" s="25">
-        <f>'Balance Sheet'!I52</f>
+        <f>'Balance Sheet'!I53</f>
         <v>-539.78442317572933</v>
       </c>
       <c r="E15" s="25">
-        <f>'Balance Sheet'!J52</f>
+        <f>'Balance Sheet'!J53</f>
         <v>-574.06719664336379</v>
       </c>
       <c r="F15" s="25">
-        <f>'Balance Sheet'!K52</f>
+        <f>'Balance Sheet'!K53</f>
         <v>-610.64026286698993</v>
       </c>
       <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="25">
         <f>-'Balance Sheet'!G12+'Balance Sheet'!F12</f>
@@ -7932,7 +8016,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="26">
         <f>SUM(B15:B18)</f>
@@ -7967,7 +8051,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
@@ -7978,7 +8062,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" s="25">
         <f>'Balance Sheet'!G22-'Balance Sheet'!F22</f>
@@ -8004,7 +8088,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B23" s="25">
         <f>'Balance Sheet'!G28-'Balance Sheet'!F28</f>
@@ -8030,7 +8114,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24" s="25">
         <f>'Balance Sheet'!G37-'Balance Sheet'!F37</f>
@@ -8056,33 +8140,33 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25" s="25">
-        <f>'Balance Sheet'!G54</f>
+        <f>'Balance Sheet'!G55</f>
         <v>-327</v>
       </c>
       <c r="C25" s="25">
-        <f>'Balance Sheet'!H54</f>
+        <f>'Balance Sheet'!H55</f>
         <v>-327</v>
       </c>
       <c r="D25" s="25">
-        <f>'Balance Sheet'!I54</f>
+        <f>'Balance Sheet'!I55</f>
         <v>-327</v>
       </c>
       <c r="E25" s="25">
-        <f>'Balance Sheet'!J54</f>
+        <f>'Balance Sheet'!J55</f>
         <v>-327</v>
       </c>
       <c r="F25" s="25">
-        <f>'Balance Sheet'!K54</f>
+        <f>'Balance Sheet'!K55</f>
         <v>-327</v>
       </c>
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B26" s="25">
         <v>288.3</v>
@@ -8103,7 +8187,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B27" s="26">
         <f>SUM(B22:B26)</f>
@@ -8138,27 +8222,27 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="26">
         <f>B27+B19+B12</f>
-        <v>-32.513645242835082</v>
+        <v>-55.318932742834932</v>
       </c>
       <c r="C29" s="26">
         <f>C27+C19+C12</f>
-        <v>-172.5315275289081</v>
+        <v>-196.7222274344258</v>
       </c>
       <c r="D29" s="26">
         <f>D27+D19+D12</f>
-        <v>-138.44101748250773</v>
+        <v>-164.09952578865978</v>
       </c>
       <c r="E29" s="26">
         <f>E27+E19+E12</f>
-        <v>-100.23949532405481</v>
+        <v>-127.45308661683771</v>
       </c>
       <c r="F29" s="26">
         <f>F27+F19+F12</f>
-        <v>-57.252544748318996</v>
+        <v>-86.113660786111041</v>
       </c>
       <c r="G29" s="12"/>
     </row>
@@ -8168,23 +8252,23 @@
       </c>
       <c r="B30" s="26">
         <f>B12+B15</f>
-        <v>252.24087665877266</v>
+        <v>229.43558915877281</v>
       </c>
       <c r="C30" s="26">
         <f t="shared" ref="C30:F30" si="2">C12+C15</f>
-        <v>280.68330148669531</v>
+        <v>256.49260158117761</v>
       </c>
       <c r="D30" s="26">
         <f t="shared" si="2"/>
-        <v>319.4228091091619</v>
+        <v>293.76430080300986</v>
       </c>
       <c r="E30" s="26">
         <f t="shared" si="2"/>
-        <v>362.53505942648576</v>
+        <v>335.32146813370287</v>
       </c>
       <c r="F30" s="26">
         <f t="shared" si="2"/>
-        <v>410.46966312219536</v>
+        <v>381.60854708440331</v>
       </c>
       <c r="G30" s="12"/>
     </row>

</xml_diff>